<commit_message>
Sources have been filled in with generated dummy data
</commit_message>
<xml_diff>
--- a/SRC/DEMO_CODE_dispatch.xlsx
+++ b/SRC/DEMO_CODE_dispatch.xlsx
@@ -5,25 +5,25 @@
   <workbookPr codeName="ЭтаКнига" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\OneDrive\Рабочий стол\SANDBOX\DEMO_CODE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\OneDrive\Рабочий стол\SANDBOX\DEMO_CODE\SRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34AE21D-6399-4C2F-8F46-733C110C251B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D137F822-3AB2-4E39-B234-26F155A04D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="823" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="823" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01.05.2023 " sheetId="3218" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'01.05.2023 '!$A$1:$J$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'01.05.2023 '!$A$1:$J$57</definedName>
   </definedNames>
   <calcPr calcId="181029" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="81">
   <si>
     <t xml:space="preserve">СВОДКА ДИСПЕТЧЕСКОЙ СЛУЖБЫ ООО "DEMO_CODE" </t>
   </si>
@@ -46,14 +46,6 @@
     <t>Пробег, тыс. км.</t>
   </si>
   <si>
-    <t>Экскурсия по городу</t>
-  </si>
-  <si>
-    <t>Автослесарь
-Родин В.С.
-тел: +7982111222</t>
-  </si>
-  <si>
     <t xml:space="preserve">Задания для автомобилей с 06:00-18:00 </t>
   </si>
   <si>
@@ -75,44 +67,7 @@
     <t>низк</t>
   </si>
   <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 42 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">59 </t>
-  </si>
-  <si>
     <t>Центральный АО</t>
-  </si>
-  <si>
-    <t>Chevrolet Camaro О 123 ЕХ 100</t>
-  </si>
-  <si>
-    <t>Chevrolet Impala О 456 ЕР 101</t>
-  </si>
-  <si>
-    <t>Chevrolet Malibu С 789 НХ 102</t>
-  </si>
-  <si>
-    <t>Chevrolet Tahoe К 321 РО 103</t>
-  </si>
-  <si>
-    <t>Chevrolet Equinox У 654 ОУ 104</t>
-  </si>
-  <si>
-    <t>Chevrolet Traverse О 987 РЕ 105</t>
-  </si>
-  <si>
-    <t>Начальник колоны
-Иванов А.С.
-тел: +7982111222</t>
-  </si>
-  <si>
-    <t>Механик 1 смены
-Смирнов В.М.
-тел: +7982111222</t>
   </si>
   <si>
     <t>Механик 2 смены
@@ -120,15 +75,251 @@
 тел: +7982111222</t>
   </si>
   <si>
+    <t>Начальник смены диспетчерской службы:   Васильев С.Д.</t>
+  </si>
+  <si>
+    <t>Технолог диспетчерской службы: Петров Г.Н.</t>
+  </si>
+  <si>
+    <t>Начальник колоны
+Иванов А.С.
+тел: +79893519221</t>
+  </si>
+  <si>
+    <t>Механик 1 смены
+Смирнов В.М.
+тел: +79892291935</t>
+  </si>
+  <si>
     <t>Автоэлектрик
 Попов Е.А.
+тел: +79891992912</t>
+  </si>
+  <si>
+    <t>Автослесарь
+Родин В.С.
+тел: +79898291922</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>Mercedes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Северный АО
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Северо-Западный АО
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Западный АО
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Юго-Западный АО
+</t>
+  </si>
+  <si>
+    <t>Chevrolet Camaro О 123 ЕХ 777</t>
+  </si>
+  <si>
+    <t>Chevrolet Impala О 456 ЕР 199</t>
+  </si>
+  <si>
+    <t>Chevrolet Malibu С 789 НХ 797</t>
+  </si>
+  <si>
+    <t>Chevrolet Tahoe К 321 РО 177</t>
+  </si>
+  <si>
+    <t>Chevrolet Equinox У 654 ОУ 799</t>
+  </si>
+  <si>
+    <t>Chevrolet Traverse О 987 РЕ 797</t>
+  </si>
+  <si>
+    <t>Chevrolet Silverado Е 456 СР 799</t>
+  </si>
+  <si>
+    <t>Toyota Corolla О 123 УХ 777</t>
+  </si>
+  <si>
+    <t>Toyota Camry Р 799 СЕ 799</t>
+  </si>
+  <si>
+    <t>Toyota RAV4 У 797 УХ 777</t>
+  </si>
+  <si>
+    <t>Toyota Prius О 777 ОР 799</t>
+  </si>
+  <si>
+    <t>Toyota Highlander Е 799 СС 797</t>
+  </si>
+  <si>
+    <t>Toyota Sienna Р 197 ОС 199</t>
+  </si>
+  <si>
+    <t>Toyota Tacoma К 199 НС 777</t>
+  </si>
+  <si>
+    <t>Ford Mustang Р 123 РХ 799</t>
+  </si>
+  <si>
+    <t>Ford F-150 О 197 СС 777</t>
+  </si>
+  <si>
+    <t>Ford Escape У 799 СС 799</t>
+  </si>
+  <si>
+    <t>Ford Explorer Р 199 ЕХ 197</t>
+  </si>
+  <si>
+    <t>Ford Fusion У 977 ЕС 199</t>
+  </si>
+  <si>
+    <t>BMW X5 О 123 УХ 799</t>
+  </si>
+  <si>
+    <t>BMW 3 Series С 456 НУ 799</t>
+  </si>
+  <si>
+    <t>BMW 5 Series О 789 РО 799</t>
+  </si>
+  <si>
+    <t>BMW X3 С 234 ОР 799</t>
+  </si>
+  <si>
+    <t>BMW 7 Series У 512 ОУ 777</t>
+  </si>
+  <si>
+    <t>BMW X7 К 888 ЕХ 799</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz C-Class У 798 ОН 799</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz E-Class К 111 УО 799</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz GLE О 123 ЕР 799</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz A-Class Р 234 ОС 799</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz S-Class У 512 УУ 799</t>
+  </si>
+  <si>
+    <t>Техническое обслуживание и ремонт</t>
+  </si>
+  <si>
+    <t>Механик 1 смены
+Петров В.А.
+тел: +79892291935</t>
+  </si>
+  <si>
+    <t>Механик 2 смены
+Николаев А.И.
 тел: +7982111222</t>
   </si>
   <si>
-    <t>Начальник смены диспетчерской службы:   Васильев С.Д.</t>
-  </si>
-  <si>
-    <t>Технолог диспетчерской службы: Петров Г.Н.</t>
+    <t>Автоэлектрик
+Морозов В.П.
+тел: +79891992912</t>
+  </si>
+  <si>
+    <t>Автослесарь
+Лебедев М.Д.
+тел: +79898291922</t>
+  </si>
+  <si>
+    <t>Начальник колоны
+Егоров И.П.
+тел: +79893519221</t>
+  </si>
+  <si>
+    <t>Механик 1 смены
+Федоров А.В.
+тел: +79892291935</t>
+  </si>
+  <si>
+    <t>Механик 2 смены
+Васильев В.Н.
+тел: +7982111222</t>
+  </si>
+  <si>
+    <t>Автоэлектрик
+Громов А.О.
+тел: +79891992912</t>
+  </si>
+  <si>
+    <t>Автослесарь
+Дмитриев В.Г.
+тел: +79898291922</t>
+  </si>
+  <si>
+    <t>Начальник колоны
+Шевченко А.Л.
+тел: +79893519221</t>
+  </si>
+  <si>
+    <t>Механик 1 смены
+Орлов А.Р.
+тел: +79892291935</t>
+  </si>
+  <si>
+    <t>Механик 2 смены
+Козлов В.Е.
+тел: +7982111222</t>
+  </si>
+  <si>
+    <t>Автоэлектрик
+Соловьев И.Н.
+тел: +79891992912</t>
+  </si>
+  <si>
+    <t>Автослесарь
+Медведев С.А.
+тел: +79898291922</t>
+  </si>
+  <si>
+    <t>Начальник колоны
+Назаров В.К.
+тел: +79893519221</t>
+  </si>
+  <si>
+    <t>Механик 1 смены
+Белов М.Т.
+тел: +79892291935</t>
+  </si>
+  <si>
+    <t>Механик 2 смены
+Горбачев А.Ю.
+тел: +7982111222</t>
+  </si>
+  <si>
+    <t>Автоэлектрик
+Савельев В.Л.
+тел: +79891992912</t>
+  </si>
+  <si>
+    <t>Автослесарь
+Фомин И.Д.
+тел: +79898291922</t>
+  </si>
+  <si>
+    <t>Начальник колоны
+Соколов М.В.
+тел: +79898919292</t>
   </si>
 </sst>
 </file>
@@ -205,14 +396,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="36"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="50"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -230,6 +413,14 @@
     <font>
       <b/>
       <sz val="45"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="42"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -263,7 +454,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -326,51 +517,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -538,6 +684,17 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -547,13 +704,50 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -562,147 +756,156 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="4" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="4" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="4" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="4" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1016,19 +1219,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Лист1">
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="18" zoomScaleNormal="24" zoomScaleSheetLayoutView="25" zoomScalePageLayoutView="20" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="46" x14ac:dyDescent="0.95"/>
   <cols>
-    <col min="1" max="1" width="71.1796875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="85.6328125" style="2" customWidth="1"/>
     <col min="2" max="2" width="39.453125" style="2" customWidth="1"/>
     <col min="3" max="3" width="210.54296875" style="2" customWidth="1"/>
     <col min="4" max="4" width="109.1796875" style="2" customWidth="1"/>
@@ -1042,46 +1245,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="1">
-      <c r="A1" s="41">
+      <c r="A1" s="32">
         <v>45047</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="46" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="48"/>
-    </row>
-    <row r="2" spans="1:10" ht="93.75" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="36"/>
+    </row>
+    <row r="2" spans="1:10" ht="94" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="44"/>
     </row>
     <row r="3" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A3" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="36"/>
+      <c r="A3" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="41"/>
       <c r="C3" s="13" t="s">
         <v>3</v>
       </c>
@@ -1107,131 +1310,131 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="104.15" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A4" s="38"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="15" t="s">
-        <v>20</v>
+    <row r="4" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A4" s="47"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="49" t="s">
+        <v>30</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="16">
-        <v>55</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>24</v>
+        <v>59</v>
+      </c>
+      <c r="G4" s="49" t="s">
+        <v>35</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="104.15" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A5" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="17" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="J4" s="16">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A5" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="41"/>
+      <c r="C5" s="50" t="s">
+        <v>31</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="30">
+        <v>83</v>
+      </c>
+      <c r="G5" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="18">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A6" s="47"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="16">
+        <v>88</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="16"/>
+    </row>
+    <row r="7" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A7" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="41"/>
+      <c r="C7" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="30">
-        <v>68</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="18">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="104.15" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A6" s="38"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="16">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="104.15" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A7" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="E7" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="F7" s="30">
+        <v>65</v>
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="19"/>
     </row>
-    <row r="8" spans="1:10" ht="104.15" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A8" s="38"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="21"/>
+    <row r="8" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A8" s="47"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="16">
+        <v>54</v>
+      </c>
       <c r="G8" s="20"/>
       <c r="H8" s="4"/>
       <c r="I8" s="3"/>
       <c r="J8" s="21"/>
     </row>
-    <row r="9" spans="1:10" ht="104.15" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A9" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="36"/>
+    <row r="9" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A9" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="41"/>
       <c r="C9" s="22"/>
       <c r="D9" s="10"/>
       <c r="E9" s="11"/>
@@ -1241,9 +1444,9 @@
       <c r="I9" s="11"/>
       <c r="J9" s="23"/>
     </row>
-    <row r="10" spans="1:10" ht="104.15" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A10" s="38"/>
-      <c r="B10" s="36"/>
+    <row r="10" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A10" s="47"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="20"/>
       <c r="D10" s="4"/>
       <c r="E10" s="3"/>
@@ -1253,11 +1456,11 @@
       <c r="I10" s="3"/>
       <c r="J10" s="21"/>
     </row>
-    <row r="11" spans="1:10" ht="104.15" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A11" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="36"/>
+    <row r="11" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A11" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="41"/>
       <c r="C11" s="24"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
@@ -1267,9 +1470,9 @@
       <c r="I11" s="12"/>
       <c r="J11" s="25"/>
     </row>
-    <row r="12" spans="1:10" ht="104.15" customHeight="1" thickBot="1" x14ac:dyDescent="1">
-      <c r="A12" s="40"/>
-      <c r="B12" s="37"/>
+    <row r="12" spans="1:10" ht="133" customHeight="1" thickBot="1" x14ac:dyDescent="1">
+      <c r="A12" s="48"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="26"/>
       <c r="D12" s="27"/>
       <c r="E12" s="28"/>
@@ -1279,40 +1482,924 @@
       <c r="I12" s="28"/>
       <c r="J12" s="29"/>
     </row>
-    <row r="13" spans="1:10" ht="128.25" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A13" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
+    <row r="13" spans="1:10" ht="94" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A13" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="44"/>
+    </row>
+    <row r="14" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A14" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="41"/>
+      <c r="C14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A15" s="47"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="16">
+        <v>68</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="16">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A16" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="41"/>
+      <c r="C16" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="30">
+        <v>49</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="18">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A17" s="47"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="16">
+        <v>75</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="16"/>
+    </row>
+    <row r="18" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A18" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="41"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="19"/>
+    </row>
+    <row r="19" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A19" s="47"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="21"/>
+    </row>
+    <row r="20" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A20" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="41"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="23"/>
+    </row>
+    <row r="21" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A21" s="47"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="21"/>
+    </row>
+    <row r="22" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A22" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="41"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="25"/>
+    </row>
+    <row r="23" spans="1:10" ht="133" customHeight="1" thickBot="1" x14ac:dyDescent="1">
+      <c r="A23" s="47"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="29"/>
+    </row>
+    <row r="24" spans="1:10" ht="94" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A24" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="44"/>
+    </row>
+    <row r="25" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A25" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="41"/>
+      <c r="C25" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A26" s="47"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="16">
+        <v>40</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J26" s="16">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A27" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="41"/>
+      <c r="C27" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="30">
+        <v>85</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="18">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A28" s="47"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="16">
+        <v>67</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" s="16">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A29" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="41"/>
+      <c r="C29" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="30">
+        <v>53</v>
+      </c>
+      <c r="G29" s="17"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="19"/>
+    </row>
+    <row r="30" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A30" s="47"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="21"/>
+    </row>
+    <row r="31" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A31" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="41"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="23"/>
+    </row>
+    <row r="32" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A32" s="47"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="21"/>
+    </row>
+    <row r="33" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A33" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="41"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="25"/>
+    </row>
+    <row r="34" spans="1:10" ht="133" customHeight="1" thickBot="1" x14ac:dyDescent="1">
+      <c r="A34" s="48"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="29"/>
+    </row>
+    <row r="35" spans="1:10" ht="94" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A35" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="44"/>
+    </row>
+    <row r="36" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A36" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="41"/>
+      <c r="C36" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A37" s="47"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="16">
+        <v>58</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J37" s="16">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A38" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="41"/>
+      <c r="C38" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="30">
+        <v>41</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J38" s="18">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A39" s="47"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="16">
+        <v>62</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J39" s="16">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A40" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="41"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="19"/>
+    </row>
+    <row r="41" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A41" s="47"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="21"/>
+    </row>
+    <row r="42" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A42" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="41"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="23"/>
+    </row>
+    <row r="43" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A43" s="47"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="21"/>
+    </row>
+    <row r="44" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A44" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="41"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="25"/>
+    </row>
+    <row r="45" spans="1:10" ht="133" customHeight="1" thickBot="1" x14ac:dyDescent="1">
+      <c r="A45" s="48"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="29"/>
+    </row>
+    <row r="46" spans="1:10" ht="94" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A46" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46" s="43"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="44"/>
+    </row>
+    <row r="47" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A47" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="41"/>
+      <c r="C47" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J47" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A48" s="47"/>
+      <c r="B48" s="41"/>
+      <c r="C48" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="16">
+        <v>55</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J48" s="16">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A49" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="41"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J49" s="18">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A50" s="47"/>
+      <c r="B50" s="41"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J50" s="16">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A51" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="41"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I51" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J51" s="30">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A52" s="47"/>
+      <c r="B52" s="41"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="21"/>
+    </row>
+    <row r="53" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A53" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="B53" s="41"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="23"/>
+    </row>
+    <row r="54" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A54" s="47"/>
+      <c r="B54" s="41"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="21"/>
+    </row>
+    <row r="55" spans="1:10" ht="133" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A55" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="B55" s="41"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="25"/>
+    </row>
+    <row r="56" spans="1:10" ht="133" customHeight="1" thickBot="1" x14ac:dyDescent="1">
+      <c r="A56" s="48"/>
+      <c r="B56" s="45"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="29"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="27"/>
+      <c r="I56" s="28"/>
+      <c r="J56" s="29"/>
+    </row>
+    <row r="57" spans="1:10" ht="94" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A57" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" s="37"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" s="39"/>
+      <c r="F57" s="39"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="39"/>
+      <c r="I57" s="39"/>
+      <c r="J57" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="44">
+    <mergeCell ref="B46:B56"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="G46:J46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B35:B45"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B24:B34"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="D57:J57"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C1:J1"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="15" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <rowBreaks count="2" manualBreakCount="2">
+    <brk id="23" max="9" man="1"/>
+    <brk id="45" max="9" man="1"/>
+  </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="10" max="217" man="1"/>
   </colBreaks>

</xml_diff>